<commit_message>
Sistema de ler tabela e retornar lista de ações
</commit_message>
<xml_diff>
--- a/Codes/data_table.xlsx
+++ b/Codes/data_table.xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Pacotes</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Nome</t>
   </si>
@@ -83,12 +80,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -317,69 +311,61 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="B2" s="1">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(A2, ""price"")"),11.07)</f>
+        <v>11.07</v>
+      </c>
+      <c r="C2" s="2">
+        <f>20%</f>
+        <v>0.2</v>
+      </c>
+      <c r="H2" s="2" t="str">
+        <f>getDividend("BCFF11")</f>
+        <v/>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(A3, ""price"")"),11.07)</f>
-        <v>11.07</v>
-      </c>
-      <c r="C3" s="3">
-        <f>20%</f>
-        <v>0.2</v>
-      </c>
-      <c r="H3" s="3" t="str">
-        <f>getDividend("BCFF11")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(A4, ""price"")"),72.99)</f>
+      <c r="B3" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(A3, ""price"")"),72.99)</f>
         <v>72.99</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
-  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Função para coletar valor patrimonial
</commit_message>
<xml_diff>
--- a/Codes/data_table.xlsx
+++ b/Codes/data_table.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -40,10 +40,16 @@
     <t>PE</t>
   </si>
   <si>
+    <t>Book value</t>
+  </si>
+  <si>
     <t>MXRF11.SA</t>
   </si>
   <si>
     <t>BCFF11.SA</t>
+  </si>
+  <si>
+    <t>SAPR4.SA</t>
   </si>
 </sst>
 </file>
@@ -339,22 +345,31 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="A2"/>
     <hyperlink r:id="rId2" ref="A3"/>
+    <hyperlink r:id="rId3" ref="A4"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>